<commit_message>
excel sheet bug fixed
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +417,259 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
+    <col width="50" customWidth="1" min="7" max="7"/>
+    <col width="50" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="30" customWidth="1" min="10" max="10"/>
+    <col width="30" customWidth="1" min="11" max="11"/>
+    <col width="30" customWidth="1" min="12" max="12"/>
+    <col width="30" customWidth="1" min="13" max="13"/>
+    <col width="30" customWidth="1" min="14" max="14"/>
+    <col width="30" customWidth="1" min="15" max="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Student Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Father's Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Mother Name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Contact Number</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Present Address</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Permanent Address</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>X Marks</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>XII Marks</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Physics Marks</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Chemistry Marks</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Maths Marks</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Percentage Marks</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>adityaprava sen</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>arup sen</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>mousumi sen</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>adityapravasen.0911@gmail.com</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>9073042220</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>rabindra pally, bramhapur</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>rabindra pally, bramhapur</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>93</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>89</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>CBSE</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>jhonny doe</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>john doe</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>jane doe</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>jhonny123@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>911</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>chicago</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>chicago</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>ISC</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>